<commit_message>
update salary and variables name such as factor_date instead history
</commit_message>
<xml_diff>
--- a/App/dist/salary/Targets/1403/02-ordibehesht.xlsx
+++ b/App/dist/salary/Targets/1403/02-ordibehesht.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="45">
   <si>
     <t xml:space="preserve">branch_id</t>
   </si>
@@ -113,9 +113,6 @@
   </si>
   <si>
     <t xml:space="preserve">شعبه قشم</t>
-  </si>
-  <si>
-    <t xml:space="preserve">داود سلامی</t>
   </si>
   <si>
     <t xml:space="preserve">طيبه فرهادي</t>
@@ -168,7 +165,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -213,6 +210,13 @@
       <name val="Samim"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -270,36 +274,40 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -376,17 +384,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20"/>
@@ -397,7 +405,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="2" width="19.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.13"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="11" style="1" width="9"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="16.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="1" width="12"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="16" style="1" width="9"/>
   </cols>
@@ -554,7 +563,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="6" t="n">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>20</v>
@@ -582,7 +591,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>208</v>
+        <v>240</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>21</v>
@@ -763,7 +772,7 @@
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="4" t="n">
-        <v>461351350.1517</v>
+        <v>1153378375</v>
       </c>
       <c r="I13" s="4" t="n">
         <v>0</v>
@@ -781,7 +790,7 @@
         <v>353</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>15</v>
@@ -791,7 +800,7 @@
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="4" t="n">
-        <v>692027025.227549</v>
+        <v>1153378375</v>
       </c>
       <c r="I14" s="4" t="n">
         <v>0</v>
@@ -799,6 +808,7 @@
       <c r="J14" s="4" t="n">
         <v>30000000</v>
       </c>
+      <c r="M14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="n">
@@ -833,13 +843,13 @@
         <v>1</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="6" t="n">
         <v>245</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>13</v>
@@ -861,13 +871,13 @@
         <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="6" t="n">
         <v>245</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>15</v>
@@ -889,13 +899,13 @@
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="6" t="n">
         <v>305</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>13</v>
@@ -917,13 +927,13 @@
         <v>1</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="6" t="n">
         <v>305</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>15</v>
@@ -945,13 +955,13 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="6" t="n">
         <v>317</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>13</v>
@@ -973,13 +983,13 @@
         <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="6" t="n">
         <v>317</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>15</v>
@@ -1001,13 +1011,13 @@
         <v>39</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="6" t="n">
         <v>281</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>13</v>
@@ -1029,13 +1039,13 @@
         <v>39</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="6" t="n">
         <v>280</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>15</v>
@@ -1057,13 +1067,13 @@
         <v>40</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24" s="6" t="n">
         <v>285</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>15</v>
@@ -1087,13 +1097,13 @@
         <v>40</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" s="6" t="n">
         <v>285</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>13</v>
@@ -1115,13 +1125,13 @@
         <v>35</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="6" t="n">
         <v>245</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>13</v>
@@ -1143,7 +1153,7 @@
         <v>35</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C27" s="6" t="n">
         <v>216</v>
@@ -1171,13 +1181,13 @@
         <v>32</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C28" s="6" t="n">
         <v>323</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>13</v>
@@ -1199,13 +1209,13 @@
         <v>32</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C29" s="6" t="n">
         <v>323</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>15</v>
@@ -1229,7 +1239,7 @@
         <v>23</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C30" s="6" t="n">
         <v>200</v>
@@ -1257,7 +1267,7 @@
         <v>23</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C31" s="6" t="n">
         <v>228</v>
@@ -1282,8 +1292,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>